<commit_message>
Reporte Mensual 30 Boleta de Pago y Validado Afp
</commit_message>
<xml_diff>
--- a/MySql/renta_quinta_rfija (3).xlsx
+++ b/MySql/renta_quinta_rfija (3).xlsx
@@ -18,10 +18,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>CONTA 1</author>
     <author>Anibal</author>
   </authors>
   <commentList>
-    <comment ref="J8" authorId="0">
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>CONTA 1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Suma de todo los ingresos afectos  Renta5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -41,11 +66,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-28 de julio</t>
+Gratificacion  proyectada 
+para Diciembre
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0">
+    <comment ref="O8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -70,7 +97,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
+    <comment ref="J9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anibal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+9% All los ingresos del mes 
+de JUNIO (3075*0.09) 
+++ php</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -92,12 +145,11 @@
           <t xml:space="preserve">
 9% de gratificacion
 q corresponde ESSALUD
-del 28 de julio
-INSERT concepto [312]</t>
+de navidad  ++PHP</t>
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0">
+    <comment ref="J12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -117,37 +169,14 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-9% de gratificacion
-q corresponde ESSALUD
-de navidad</t>
+DE 28- esto ah variado xq
+tiene una gratificacion proporcinal !!! OK 
+OPERACIÓN UNICA A
+F=(3075 /6 meses) * 4 meses q laboro. Ojo si Mes trabaja el 1ero el mes es valido para multiplicar.Sino pasa al siguiente mes PHP !</t>
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Anibal:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DE 28</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
+    <comment ref="K13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -176,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>enero</t>
   </si>
@@ -372,9 +401,6 @@
     <t>Exeso de 54UIT</t>
   </si>
   <si>
-    <t>Tasa progresiva acumulativa</t>
-  </si>
-  <si>
     <t>Hasta 27UIT</t>
   </si>
   <si>
@@ -423,12 +449,51 @@
   <si>
     <t>Mejor calc despues de generar Mensual.</t>
   </si>
+  <si>
+    <t>Tasas progresivas acumulativas</t>
+  </si>
+  <si>
+    <t>ah pagado</t>
+  </si>
+  <si>
+    <t>proporcional</t>
+  </si>
+  <si>
+    <t>3075*0.09=276.75  no sera monto de julio sino proporcinal =2050  = 2050*0.09= 184.5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GRATIFICACION PROPORCIONAL (resta de junio = todo ingreso =3075) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2050</t>
+    </r>
+  </si>
+  <si>
+    <t>ID10</t>
+  </si>
+  <si>
+    <t>TODOS LOS ingresos + 9%</t>
+  </si>
+  <si>
+    <t>3075*0.09=276.75</t>
+  </si>
+  <si>
+    <t>3075+276.75=  3351.75</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,8 +536,36 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,8 +656,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -668,11 +779,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -699,7 +821,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -709,7 +830,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -725,6 +845,36 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +883,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF66FF"/>
       <color rgb="FFFED6FF"/>
-      <color rgb="FFFF66FF"/>
       <color rgb="FFFF9F9F"/>
     </mruColors>
   </colors>
@@ -1026,15 +1176,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="46" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
@@ -1045,7 +1196,10 @@
     <col min="15" max="15" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
+      <c r="A1" s="47" t="s">
+        <v>55</v>
+      </c>
       <c r="B1" t="s">
         <v>32</v>
       </c>
@@ -1055,13 +1209,16 @@
       <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="B2" s="30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="I1" s="54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1237,7 @@
       <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="33" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1095,410 +1252,469 @@
       <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75">
+      <c r="P4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16.5">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="E5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="F5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="G5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="H5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="I5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="J5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="K5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="L5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="M5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="N5" s="47">
-        <v>2067.5</v>
-      </c>
-      <c r="O5" s="47">
-        <v>2067.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="D5" s="45">
+        <v>0</v>
+      </c>
+      <c r="E5" s="45">
+        <v>2333.33</v>
+      </c>
+      <c r="F5" s="45">
+        <v>3067.5</v>
+      </c>
+      <c r="G5" s="45">
+        <v>3067.5</v>
+      </c>
+      <c r="H5" s="45">
+        <v>3067.5</v>
+      </c>
+      <c r="I5" s="56">
+        <v>3075</v>
+      </c>
+      <c r="J5" s="58">
+        <v>5401.75</v>
+      </c>
+      <c r="K5" s="45">
+        <v>3075</v>
+      </c>
+      <c r="L5" s="45">
+        <v>3075</v>
+      </c>
+      <c r="M5" s="45">
+        <v>3075</v>
+      </c>
+      <c r="N5" s="56">
+        <v>3075</v>
+      </c>
+      <c r="O5" s="58">
+        <v>3351.75</v>
+      </c>
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="46">
+        <v>2</v>
+      </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>12</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>11</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>10</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="27">
         <v>9</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <v>8</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="27">
         <v>7</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <v>6</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="27">
         <v>5</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <v>4</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="27">
         <v>3</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="27">
         <v>2</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1">
+    <row r="7" spans="1:17" s="2" customFormat="1">
+      <c r="A7" s="47">
+        <v>3</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
-        <v>24810</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ref="E7:O7" si="0">E5*E6</f>
-        <v>22742.5</v>
+        <v>25666.629999999997</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>20675</v>
+        <v>30675</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>18607.5</v>
+        <v>27607.5</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>16540</v>
+        <v>24540</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>14472.5</v>
+        <v>21525</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>12405</v>
+        <v>32410.5</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
-        <v>10337.5</v>
+        <v>15375</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="0"/>
-        <v>8270</v>
+        <v>12300</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="0"/>
-        <v>6202.5</v>
+        <v>9225</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>4135</v>
+        <v>6150</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="0"/>
-        <v>2067.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="30"/>
+        <v>3351.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="48">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="32">
         <f>D5*2</f>
-        <v>4135</v>
-      </c>
-      <c r="E8" s="34">
-        <f t="shared" ref="E8:G8" si="1">E5*2</f>
-        <v>4135</v>
-      </c>
-      <c r="F8" s="34">
-        <f t="shared" si="1"/>
-        <v>4135</v>
-      </c>
-      <c r="G8" s="34">
-        <f t="shared" si="1"/>
-        <v>4135</v>
-      </c>
-      <c r="H8" s="34">
+        <v>0</v>
+      </c>
+      <c r="E8" s="32">
+        <f>E5*2</f>
+        <v>4666.66</v>
+      </c>
+      <c r="F8" s="32">
+        <f>F5*2</f>
+        <v>6135</v>
+      </c>
+      <c r="G8" s="32">
+        <f t="shared" ref="G8" si="1">G5*2</f>
+        <v>6135</v>
+      </c>
+      <c r="H8" s="32">
         <f>H5*2</f>
-        <v>4135</v>
-      </c>
-      <c r="I8" s="34">
+        <v>6135</v>
+      </c>
+      <c r="I8" s="32">
         <f>I5*2</f>
-        <v>4135</v>
-      </c>
-      <c r="J8" s="6">
-        <f>J5*1</f>
-        <v>2067.5</v>
+        <v>6150</v>
+      </c>
+      <c r="J8" s="55">
+        <v>5401.75</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" ref="K8:O8" si="2">K5*1</f>
-        <v>2067.5</v>
+        <f>K5*1</f>
+        <v>3075</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="2"/>
-        <v>2067.5</v>
+        <f t="shared" ref="L8:O8" si="2">L5*1</f>
+        <v>3075</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="2"/>
-        <v>2067.5</v>
+        <v>3075</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
-        <v>2067.5</v>
+        <v>3075</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="2"/>
-        <v>2067.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>3351.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="46">
+        <v>5</v>
+      </c>
       <c r="B9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9">
-        <f>J8*0.09</f>
-        <v>186.07499999999999</v>
-      </c>
-      <c r="K9" s="31"/>
+      <c r="J9" s="54">
+        <f>I5*0.09</f>
+        <v>276.75</v>
+      </c>
+      <c r="K9" s="30"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="32">
-        <f>O8*0.09</f>
-        <v>186.07499999999999</v>
+      <c r="O9" s="61">
+        <f>N5*0.09</f>
+        <v>276.75</v>
       </c>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" s="5" customFormat="1">
+    <row r="10" spans="1:17" s="5" customFormat="1">
+      <c r="A10" s="47">
+        <v>6</v>
+      </c>
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="5">
         <f>D7+D8+D9</f>
-        <v>28945</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
         <f>E7+E8+E9</f>
-        <v>26877.5</v>
+        <v>30333.289999999997</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ref="F10:O10" si="3">F7+F8+F9</f>
-        <v>24810</v>
+        <v>36810</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>22742.5</v>
+        <v>33742.5</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="3"/>
-        <v>20675</v>
+        <v>30675</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="3"/>
-        <v>18607.5</v>
+        <v>27675</v>
       </c>
       <c r="J10" s="5">
         <f>J7+J8+J9</f>
-        <v>14658.575000000001</v>
+        <v>38089</v>
       </c>
       <c r="K10" s="5">
         <f>K7+K8+K9</f>
-        <v>12405</v>
+        <v>18450</v>
       </c>
       <c r="L10" s="5">
         <f>L7+L8+L9</f>
-        <v>10337.5</v>
+        <v>15375</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="3"/>
-        <v>8270</v>
+        <v>12300</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="3"/>
-        <v>6202.5</v>
+        <v>9225</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="3"/>
-        <v>4321.0749999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>6980.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="46">
+        <v>7</v>
+      </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="7">
         <f>D5</f>
-        <v>2067.5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="7">
         <f>SUM(D5+E5)</f>
-        <v>4135</v>
+        <v>2333.33</v>
       </c>
       <c r="G11" s="7">
-        <f>(E5+F5+G5)</f>
-        <v>6202.5</v>
+        <f>(E5+F5+D5)</f>
+        <v>5400.83</v>
       </c>
       <c r="H11">
         <f>D5+E5+F5+G5</f>
-        <v>8270</v>
+        <v>8468.33</v>
       </c>
       <c r="I11">
         <f>D5+E5+F5+G5+H5</f>
-        <v>10337.5</v>
+        <v>11535.83</v>
       </c>
       <c r="J11">
         <f>D5+E5+F5+G5+H5+I5</f>
-        <v>12405</v>
+        <v>14610.83</v>
       </c>
       <c r="K11">
         <f>D5+E5+F5+G5+H5+I5+J5</f>
-        <v>14472.5</v>
+        <v>20012.580000000002</v>
       </c>
       <c r="L11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5</f>
-        <v>16540</v>
+        <v>23087.58</v>
       </c>
       <c r="M11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5</f>
-        <v>18607.5</v>
+        <v>26162.58</v>
       </c>
       <c r="N11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5+M5</f>
-        <v>20675</v>
+        <v>29237.58</v>
       </c>
       <c r="O11" s="17">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5</f>
-        <v>22742.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="30"/>
+        <v>32312.58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A12" s="48">
+        <v>8</v>
+      </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="34">
-        <f>J8</f>
-        <v>2067.5</v>
-      </c>
-      <c r="K12" s="34">
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="59">
+        <v>2050</v>
+      </c>
+      <c r="K12" s="32">
         <f>J12</f>
-        <v>2067.5</v>
-      </c>
-      <c r="L12" s="34">
-        <f t="shared" ref="L12:O12" si="4">K12</f>
-        <v>2067.5</v>
-      </c>
-      <c r="M12" s="34">
+        <v>2050</v>
+      </c>
+      <c r="L12" s="32">
+        <f>K12</f>
+        <v>2050</v>
+      </c>
+      <c r="M12" s="32">
+        <f t="shared" ref="M12:O12" si="4">L12</f>
+        <v>2050</v>
+      </c>
+      <c r="N12" s="32">
         <f t="shared" si="4"/>
-        <v>2067.5</v>
-      </c>
-      <c r="N12" s="34">
+        <v>2050</v>
+      </c>
+      <c r="O12" s="60">
         <f t="shared" si="4"/>
-        <v>2067.5</v>
-      </c>
-      <c r="O12" s="34">
-        <f t="shared" si="4"/>
-        <v>2067.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="30">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30">
+      <c r="A13" s="46">
+        <v>9</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="38">
         <f>J9</f>
-        <v>186.07499999999999</v>
+        <v>276.75</v>
       </c>
       <c r="L13">
         <f>J9</f>
-        <v>186.07499999999999</v>
+        <v>276.75</v>
       </c>
       <c r="M13">
         <f>J9</f>
-        <v>186.07499999999999</v>
+        <v>276.75</v>
       </c>
       <c r="N13">
         <f>J9</f>
-        <v>186.07499999999999</v>
+        <v>276.75</v>
       </c>
       <c r="O13">
         <f>J9</f>
-        <v>186.07499999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>276.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="46">
+        <v>10</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
+      <c r="A15" s="46">
+        <v>11</v>
+      </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
+      <c r="A16" s="46">
+        <v>12</v>
+      </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="46">
+        <v>13</v>
+      </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="1:15">
+      <c r="A18" s="46">
+        <v>14</v>
+      </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="1:15">
+      <c r="A19" s="46">
+        <v>15</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1513,68 +1729,77 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="26"/>
-    </row>
-    <row r="20" spans="2:15" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="49">
+        <v>16</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="27"/>
-    </row>
-    <row r="21" spans="2:15" s="5" customFormat="1">
+      <c r="O20" s="26"/>
+    </row>
+    <row r="21" spans="1:15" s="5" customFormat="1">
+      <c r="A21" s="47">
+        <v>17</v>
+      </c>
       <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="5">
         <f>SUM(D10:D20)</f>
-        <v>28945</v>
+        <v>0</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" ref="E21:O21" si="5">SUM(E10:E20)</f>
-        <v>28945</v>
+        <v>30333.289999999997</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="5"/>
-        <v>28945</v>
+        <v>39143.33</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="5"/>
-        <v>28945</v>
+        <v>39143.33</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="5"/>
-        <v>28945</v>
+        <v>39143.33</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="5"/>
-        <v>28945</v>
+        <v>39210.83</v>
       </c>
       <c r="J21" s="5">
         <f>SUM(J10:J20)</f>
-        <v>29131.075000000001</v>
+        <v>54749.83</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="5"/>
-        <v>29131.075000000001</v>
+        <v>40789.33</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="5"/>
-        <v>29131.075000000001</v>
+        <v>40789.33</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>29131.075000000001</v>
+        <v>40789.33</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="5"/>
-        <v>29131.075000000001</v>
+        <v>40789.33</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="5"/>
-        <v>29317.15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15">
+        <v>41619.58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="46">
+        <v>18</v>
+      </c>
       <c r="B22" t="s">
         <v>27</v>
       </c>
@@ -1631,447 +1856,506 @@
         <v>25550</v>
       </c>
     </row>
-    <row r="23" spans="2:15" s="5" customFormat="1">
+    <row r="23" spans="1:15" s="5" customFormat="1">
+      <c r="A23" s="47">
+        <v>19</v>
+      </c>
       <c r="B23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="39">
         <f>D21-D22</f>
-        <v>3395</v>
+        <v>-25550</v>
       </c>
       <c r="E23" s="5">
         <f>E21-E22</f>
-        <v>3395</v>
+        <v>4783.2899999999972</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ref="F23:O23" si="6">F21-F22</f>
-        <v>3395</v>
+        <v>13593.330000000002</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="6"/>
-        <v>3395</v>
+        <v>13593.330000000002</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="6"/>
-        <v>3395</v>
+        <v>13593.330000000002</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" si="6"/>
-        <v>3395</v>
+        <v>13660.830000000002</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="6"/>
-        <v>3581.0750000000007</v>
+        <v>29199.83</v>
       </c>
       <c r="K23" s="5">
         <f>K21-K22</f>
-        <v>3581.0750000000007</v>
+        <v>15239.330000000002</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="6"/>
-        <v>3581.0750000000007</v>
+        <v>15239.330000000002</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="6"/>
-        <v>3581.0750000000007</v>
+        <v>15239.330000000002</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="6"/>
-        <v>3581.0750000000007</v>
+        <v>15239.330000000002</v>
       </c>
       <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>3767.1500000000015</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15">
+        <v>16069.580000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="46">
+        <v>20</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="2:15">
-      <c r="B25" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="39">
+      <c r="C25" s="37">
         <v>0.15</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="38">
         <f>IF(D23&gt;0,(D23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="E25" s="40">
+        <v>0</v>
+      </c>
+      <c r="E25" s="38">
         <f>IF(E23&gt;0,(E23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="F25" s="40">
+        <v>717.49349999999959</v>
+      </c>
+      <c r="F25" s="38">
         <f>IF(F23&gt;0,(F23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="G25" s="40">
+        <v>2038.9995000000001</v>
+      </c>
+      <c r="G25" s="38">
         <f>IF(G23&gt;0,(G23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="H25" s="40">
+        <v>2038.9995000000001</v>
+      </c>
+      <c r="H25" s="38">
         <f>IF(H23&gt;0,(H23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="I25" s="40">
+        <v>2038.9995000000001</v>
+      </c>
+      <c r="I25" s="38">
         <f>IF(I23&gt;0,(I23*C25),0)</f>
-        <v>509.25</v>
-      </c>
-      <c r="J25" s="40">
+        <v>2049.1245000000004</v>
+      </c>
+      <c r="J25" s="38">
         <f>IF(J23&gt;0,(J23*C25),0)</f>
-        <v>537.16125000000011</v>
-      </c>
-      <c r="K25" s="40">
+        <v>4379.9745000000003</v>
+      </c>
+      <c r="K25" s="38">
         <f>IF(K23&gt;0,(K23*C25),0)</f>
-        <v>537.16125000000011</v>
-      </c>
-      <c r="L25" s="40">
+        <v>2285.8995</v>
+      </c>
+      <c r="L25" s="38">
         <f>IF(L23&gt;0,(L23*C25),0)</f>
-        <v>537.16125000000011</v>
-      </c>
-      <c r="M25" s="40">
+        <v>2285.8995</v>
+      </c>
+      <c r="M25" s="38">
         <f>IF(M23&gt;0,(M23*C25),0)</f>
-        <v>537.16125000000011</v>
-      </c>
-      <c r="N25" s="40">
+        <v>2285.8995</v>
+      </c>
+      <c r="N25" s="38">
         <f>IF(N23&gt;0,(N23*C25),0)</f>
-        <v>537.16125000000011</v>
-      </c>
-      <c r="O25" s="40">
+        <v>2285.8995</v>
+      </c>
+      <c r="O25" s="38">
         <f>IF(O23&gt;0,(O23*C25),0)</f>
-        <v>565.07250000000022</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
+        <v>2410.4370000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="B26" s="16"/>
-      <c r="C26" s="38" t="s">
-        <v>49</v>
+      <c r="C26" s="36" t="s">
+        <v>48</v>
       </c>
       <c r="D26" s="23"/>
       <c r="O26"/>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="1:15">
+      <c r="A27" s="46">
+        <v>21</v>
+      </c>
       <c r="B27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="38">
+        <v>39</v>
+      </c>
+      <c r="C27" s="36">
         <v>0.21</v>
       </c>
       <c r="D27" s="23"/>
       <c r="O27"/>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="1:15">
       <c r="B28" s="16"/>
       <c r="C28" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O28"/>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="1:15">
+      <c r="A29" s="46">
+        <v>22</v>
+      </c>
       <c r="B29" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="36">
         <v>0.3</v>
       </c>
       <c r="D29" s="23"/>
     </row>
-    <row r="30" spans="2:15" s="1" customFormat="1">
+    <row r="30" spans="1:15" s="1" customFormat="1">
+      <c r="A30" s="46"/>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1">
         <f>ROUND(D25+D27+D29,2)</f>
-        <v>509.25</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
         <f>ROUND(E25,2)</f>
-        <v>509.25</v>
+        <v>717.49</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ref="F30:M30" si="7">ROUND(F25,2)</f>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="7"/>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="7"/>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="7"/>
-        <v>509.25</v>
+        <v>2049.12</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="7"/>
-        <v>537.16</v>
+        <v>4379.97</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" si="7"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="7"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="M30" s="1">
         <f t="shared" si="7"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" ref="N30:O30" si="8">N25</f>
-        <v>537.16125000000011</v>
+        <v>2285.8995</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" si="8"/>
-        <v>565.07250000000022</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" s="1" customFormat="1">
+        <v>2410.4370000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="1" customFormat="1">
+      <c r="A32" s="46">
+        <v>23</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="1">
         <f>D30</f>
-        <v>509.25</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" ref="E32:O32" si="9">E30</f>
-        <v>509.25</v>
+        <v>717.49</v>
       </c>
       <c r="F32" s="1">
         <f>F30</f>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="G32" s="1">
         <f>G30</f>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="9"/>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="9"/>
-        <v>509.25</v>
+        <v>2049.12</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="9"/>
-        <v>537.16</v>
+        <v>4379.97</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="9"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="9"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="M32" s="1">
         <f t="shared" si="9"/>
-        <v>537.16</v>
+        <v>2285.9</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" si="9"/>
-        <v>537.16125000000011</v>
+        <v>2285.8995</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="9"/>
-        <v>565.07250000000022</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+        <f>O30</f>
+        <v>2410.4370000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="46">
+        <v>24</v>
+      </c>
       <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="37">
+        <v>43</v>
+      </c>
+      <c r="G34" s="35">
         <f>ROUND(D37+E37+F37,2)</f>
-        <v>127.32</v>
-      </c>
-      <c r="H34" s="42">
+        <v>229.71</v>
+      </c>
+      <c r="H34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>169.76</v>
-      </c>
-      <c r="I34" s="42">
+        <v>430.74</v>
+      </c>
+      <c r="I34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>169.76</v>
-      </c>
-      <c r="J34" s="42">
+        <v>430.74</v>
+      </c>
+      <c r="J34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>169.76</v>
-      </c>
-      <c r="K34" s="44">
+        <v>430.74</v>
+      </c>
+      <c r="K34" s="42">
         <f>ROUND(G34+J34,2)</f>
-        <v>297.08</v>
-      </c>
-      <c r="L34" s="33">
+        <v>660.45</v>
+      </c>
+      <c r="L34" s="31">
         <f>K34+K37</f>
-        <v>345.09999999999997</v>
-      </c>
-      <c r="M34" s="33">
+        <v>985.54</v>
+      </c>
+      <c r="M34" s="31">
         <f>K34+K37</f>
-        <v>345.09999999999997</v>
-      </c>
-      <c r="N34" s="33">
+        <v>985.54</v>
+      </c>
+      <c r="N34" s="31">
         <f>K34+K37</f>
-        <v>345.09999999999997</v>
-      </c>
-      <c r="O34" s="45">
+        <v>985.54</v>
+      </c>
+      <c r="O34" s="43">
         <f>D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37</f>
-        <v>492.64999999999992</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="8" customFormat="1">
+        <v>2628.08</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="8" customFormat="1">
+      <c r="A35" s="50">
+        <v>25</v>
+      </c>
       <c r="B35" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="8">
         <f>D32</f>
-        <v>509.25</v>
+        <v>0</v>
       </c>
       <c r="E35" s="8">
         <f t="shared" ref="E35:F35" si="10">E32</f>
-        <v>509.25</v>
+        <v>717.49</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="10"/>
-        <v>509.25</v>
+        <v>2039</v>
       </c>
       <c r="G35" s="8">
         <f>ROUND(G32-G34,2)</f>
-        <v>381.93</v>
+        <v>1809.29</v>
       </c>
       <c r="H35" s="8">
         <f>ROUND(H32-H34,2)</f>
-        <v>339.49</v>
+        <v>1608.26</v>
       </c>
       <c r="I35" s="8">
         <f>ROUND(I32-I34,2)</f>
-        <v>339.49</v>
+        <v>1618.38</v>
       </c>
       <c r="J35" s="8">
         <f t="shared" ref="J35:O35" si="11">ROUND(J32-J34,2)</f>
-        <v>367.4</v>
+        <v>3949.23</v>
       </c>
       <c r="K35" s="8">
-        <f t="shared" si="11"/>
-        <v>240.08</v>
+        <f>ROUND(K32-K34,2)</f>
+        <v>1625.45</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" si="11"/>
-        <v>192.06</v>
+        <v>1300.3599999999999</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" si="11"/>
-        <v>192.06</v>
+        <v>1300.3599999999999</v>
       </c>
       <c r="N35" s="8">
-        <f t="shared" si="11"/>
-        <v>192.06</v>
+        <f>ROUND(N32-N34,2)</f>
+        <v>1300.3599999999999</v>
       </c>
       <c r="O35" s="8">
-        <f t="shared" si="11"/>
-        <v>72.42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="23" customFormat="1">
+        <f>ROUND(O34-O32,2)</f>
+        <v>217.64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="23" customFormat="1">
+      <c r="A36" s="51">
+        <v>26</v>
+      </c>
       <c r="B36" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="28">
+        <v>44</v>
+      </c>
+      <c r="D36" s="27">
         <v>12</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="27">
         <v>12</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="27">
         <v>12</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G36" s="27">
         <v>9</v>
       </c>
-      <c r="H36" s="28">
+      <c r="H36" s="27">
         <v>8</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I36" s="27">
         <v>8</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36" s="27">
         <v>8</v>
       </c>
-      <c r="K36" s="28">
+      <c r="K36" s="27">
         <v>5</v>
       </c>
-      <c r="L36" s="28">
+      <c r="L36" s="27">
         <v>4</v>
       </c>
-      <c r="M36" s="28">
+      <c r="M36" s="27">
         <v>4</v>
       </c>
-      <c r="N36" s="28">
+      <c r="N36" s="27">
         <v>4</v>
       </c>
-      <c r="O36" s="29">
+      <c r="O36" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="25" customFormat="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="43">
+    <row r="37" spans="1:16" s="24" customFormat="1">
+      <c r="A37" s="52">
+        <v>27</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="41">
         <f>ROUND(D35/D36,2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="E37" s="43">
+        <v>0</v>
+      </c>
+      <c r="E37" s="41">
         <f>ROUND(E35/E36,2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="F37" s="43">
+        <v>59.79</v>
+      </c>
+      <c r="F37" s="41">
         <f>ROUND(F35/F36,2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="G37" s="25">
+        <v>169.92</v>
+      </c>
+      <c r="G37" s="24">
         <f>ROUND((G35/G36),2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="H37" s="25">
+        <v>201.03</v>
+      </c>
+      <c r="H37" s="24">
         <f>ROUND((H35/H36),2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="I37" s="25">
-        <f t="shared" ref="I37:O37" si="12">ROUND((I35/I36),2)</f>
-        <v>42.44</v>
-      </c>
-      <c r="J37" s="25">
+        <v>201.03</v>
+      </c>
+      <c r="I37" s="24">
+        <f>ROUND((I35/I36),2)</f>
+        <v>202.3</v>
+      </c>
+      <c r="J37" s="24">
+        <f t="shared" ref="J37:O37" si="12">ROUND((J35/J36),2)</f>
+        <v>493.65</v>
+      </c>
+      <c r="K37" s="44">
         <f t="shared" si="12"/>
-        <v>45.93</v>
-      </c>
-      <c r="K37" s="46">
+        <v>325.08999999999997</v>
+      </c>
+      <c r="L37" s="24">
         <f t="shared" si="12"/>
-        <v>48.02</v>
-      </c>
-      <c r="L37" s="25">
+        <v>325.08999999999997</v>
+      </c>
+      <c r="M37" s="24">
         <f t="shared" si="12"/>
-        <v>48.02</v>
-      </c>
-      <c r="M37" s="25">
+        <v>325.08999999999997</v>
+      </c>
+      <c r="N37" s="24">
         <f t="shared" si="12"/>
-        <v>48.02</v>
-      </c>
-      <c r="N37" s="25">
+        <v>325.08999999999997</v>
+      </c>
+      <c r="O37" s="24">
         <f t="shared" si="12"/>
-        <v>48.02</v>
-      </c>
-      <c r="O37" s="25">
-        <f t="shared" si="12"/>
-        <v>72.42</v>
+        <v>217.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="G39" s="53">
+        <v>4</v>
+      </c>
+      <c r="H39" s="53">
+        <v>5</v>
+      </c>
+      <c r="I39">
+        <v>6</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39" s="53">
+        <v>8</v>
+      </c>
+      <c r="L39" s="53">
+        <v>9</v>
+      </c>
+      <c r="M39" s="53">
+        <v>10</v>
+      </c>
+      <c r="N39" s="53">
+        <v>11</v>
+      </c>
+      <c r="O39" s="43">
+        <v>12</v>
+      </c>
+      <c r="P39" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2111,7 +2395,7 @@
         <v>34</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="19"/>
     </row>

</xml_diff>

<commit_message>
15 y vacacion mensual testing 1
</commit_message>
<xml_diff>
--- a/MySql/renta_quinta_rfija (3).xlsx
+++ b/MySql/renta_quinta_rfija (3).xlsx
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>enero</t>
   </si>
@@ -314,9 +314,6 @@
   </si>
   <si>
     <t>Participacion en las utilidades</t>
-  </si>
-  <si>
-    <t>Ejercicio 2012</t>
   </si>
   <si>
     <t>Renta Neta</t>
@@ -447,9 +444,6 @@
     <t>Residu</t>
   </si>
   <si>
-    <t>Mejor calc despues de generar Mensual.</t>
-  </si>
-  <si>
     <t>Tasas progresivas acumulativas</t>
   </si>
   <si>
@@ -487,6 +481,12 @@
   </si>
   <si>
     <t>3075+276.75=  3351.75</t>
+  </si>
+  <si>
+    <t>Ejercicio 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INGRESOS: IMELDA </t>
   </si>
 </sst>
 </file>
@@ -670,12 +670,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -790,11 +790,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -869,12 +882,18 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,11 +1195,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O34" sqref="O34"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1196,12 +1215,12 @@
     <col min="15" max="15" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
@@ -1210,15 +1229,15 @@
         <v>30</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,19 +1274,19 @@
       <c r="O3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3" s="56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="P4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="16.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="16.5">
       <c r="A5" s="46">
         <v>1</v>
       </c>
@@ -1275,46 +1294,46 @@
         <v>13</v>
       </c>
       <c r="D5" s="45">
-        <v>0</v>
+        <v>3150</v>
       </c>
       <c r="E5" s="45">
-        <v>2333.33</v>
+        <v>3150</v>
       </c>
       <c r="F5" s="45">
-        <v>3067.5</v>
+        <v>3150</v>
       </c>
       <c r="G5" s="45">
-        <v>3067.5</v>
+        <v>3150</v>
       </c>
       <c r="H5" s="45">
-        <v>3067.5</v>
-      </c>
-      <c r="I5" s="56">
-        <v>3075</v>
-      </c>
-      <c r="J5" s="58">
-        <v>5401.75</v>
+        <v>3150</v>
+      </c>
+      <c r="I5" s="45">
+        <v>3150</v>
+      </c>
+      <c r="J5" s="45">
+        <v>3150</v>
       </c>
       <c r="K5" s="45">
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="L5" s="45">
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="M5" s="45">
-        <v>3075</v>
-      </c>
-      <c r="N5" s="56">
-        <v>3075</v>
-      </c>
-      <c r="O5" s="58">
-        <v>3351.75</v>
+        <v>3150</v>
+      </c>
+      <c r="N5" s="45">
+        <v>3150</v>
+      </c>
+      <c r="O5" s="45">
+        <v>3150</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="46">
         <v>2</v>
       </c>
@@ -1358,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="2" customFormat="1">
+    <row r="7" spans="1:18" s="2" customFormat="1">
       <c r="A7" s="47">
         <v>3</v>
       </c>
@@ -1367,54 +1386,54 @@
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
-        <v>0</v>
+        <v>37800</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ref="E7:O7" si="0">E5*E6</f>
-        <v>25666.629999999997</v>
+        <v>34650</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>30675</v>
+        <v>31500</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>27607.5</v>
+        <v>28350</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>24540</v>
+        <v>25200</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>21525</v>
+        <v>22050</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>32410.5</v>
+        <v>18900</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
-        <v>15375</v>
+        <v>15750</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="0"/>
-        <v>12300</v>
+        <v>12600</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="0"/>
-        <v>9225</v>
+        <v>9450</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>6150</v>
+        <v>6300</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="0"/>
-        <v>3351.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="48">
         <v>4</v>
       </c>
@@ -1423,58 +1442,58 @@
       </c>
       <c r="D8" s="32">
         <f>D5*2</f>
-        <v>0</v>
+        <v>6300</v>
       </c>
       <c r="E8" s="32">
         <f>E5*2</f>
-        <v>4666.66</v>
+        <v>6300</v>
       </c>
       <c r="F8" s="32">
         <f>F5*2</f>
-        <v>6135</v>
+        <v>6300</v>
       </c>
       <c r="G8" s="32">
         <f t="shared" ref="G8" si="1">G5*2</f>
-        <v>6135</v>
+        <v>6300</v>
       </c>
       <c r="H8" s="32">
         <f>H5*2</f>
-        <v>6135</v>
+        <v>6300</v>
       </c>
       <c r="I8" s="32">
         <f>I5*2</f>
-        <v>6150</v>
+        <v>6300</v>
       </c>
       <c r="J8" s="55">
         <v>5401.75</v>
       </c>
       <c r="K8" s="6">
         <f>K5*1</f>
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ref="L8:O8" si="2">L5*1</f>
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="2"/>
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
-        <v>3075</v>
+        <v>3150</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="2"/>
-        <v>3351.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="46">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1483,19 +1502,19 @@
       <c r="I9" s="7"/>
       <c r="J9" s="54">
         <f>I5*0.09</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="61">
+      <c r="O9" s="59">
         <f>N5*0.09</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:17" s="5" customFormat="1">
+    <row r="10" spans="1:18" s="5" customFormat="1">
       <c r="A10" s="47">
         <v>6</v>
       </c>
@@ -1504,54 +1523,54 @@
       </c>
       <c r="D10" s="5">
         <f>D7+D8+D9</f>
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="E10" s="5">
         <f>E7+E8+E9</f>
-        <v>30333.289999999997</v>
+        <v>40950</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ref="F10:O10" si="3">F7+F8+F9</f>
-        <v>36810</v>
+        <v>37800</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>33742.5</v>
+        <v>34650</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="3"/>
-        <v>30675</v>
+        <v>31500</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="3"/>
-        <v>27675</v>
+        <v>28350</v>
       </c>
       <c r="J10" s="5">
         <f>J7+J8+J9</f>
-        <v>38089</v>
+        <v>24585.25</v>
       </c>
       <c r="K10" s="5">
         <f>K7+K8+K9</f>
-        <v>18450</v>
+        <v>18900</v>
       </c>
       <c r="L10" s="5">
         <f>L7+L8+L9</f>
-        <v>15375</v>
+        <v>15750</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="3"/>
-        <v>12300</v>
+        <v>12600</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="3"/>
-        <v>9225</v>
+        <v>9450</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="3"/>
-        <v>6980.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>6583.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="46">
         <v>7</v>
       </c>
@@ -1560,50 +1579,50 @@
       </c>
       <c r="E11" s="7">
         <f>D5</f>
-        <v>0</v>
+        <v>3150</v>
       </c>
       <c r="F11" s="7">
         <f>SUM(D5+E5)</f>
-        <v>2333.33</v>
+        <v>6300</v>
       </c>
       <c r="G11" s="7">
         <f>(E5+F5+D5)</f>
-        <v>5400.83</v>
+        <v>9450</v>
       </c>
       <c r="H11">
         <f>D5+E5+F5+G5</f>
-        <v>8468.33</v>
+        <v>12600</v>
       </c>
       <c r="I11">
         <f>D5+E5+F5+G5+H5</f>
-        <v>11535.83</v>
+        <v>15750</v>
       </c>
       <c r="J11">
         <f>D5+E5+F5+G5+H5+I5</f>
-        <v>14610.83</v>
+        <v>18900</v>
       </c>
       <c r="K11">
         <f>D5+E5+F5+G5+H5+I5+J5</f>
-        <v>20012.580000000002</v>
+        <v>22050</v>
       </c>
       <c r="L11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5</f>
-        <v>23087.58</v>
+        <v>25200</v>
       </c>
       <c r="M11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5</f>
-        <v>26162.58</v>
+        <v>28350</v>
       </c>
       <c r="N11">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5+M5</f>
-        <v>29237.58</v>
+        <v>31500</v>
       </c>
       <c r="O11" s="17">
         <f>D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5</f>
-        <v>32312.58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="16.5" thickBot="1">
+        <v>34650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16.5" thickBot="1">
       <c r="A12" s="48">
         <v>8</v>
       </c>
@@ -1611,12 +1630,12 @@
         <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="59">
+        <v>49</v>
+      </c>
+      <c r="J12" s="57">
         <v>2050</v>
       </c>
       <c r="K12" s="32">
@@ -1635,12 +1654,12 @@
         <f t="shared" si="4"/>
         <v>2050</v>
       </c>
-      <c r="O12" s="60">
+      <c r="O12" s="58">
         <f t="shared" si="4"/>
         <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="30">
+    <row r="13" spans="1:18" ht="30">
       <c r="A13" s="46">
         <v>9</v>
       </c>
@@ -1649,26 +1668,26 @@
       </c>
       <c r="K13" s="38">
         <f>J9</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="L13">
         <f>J9</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="M13">
         <f>J9</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="N13">
         <f>J9</f>
-        <v>276.75</v>
+        <v>283.5</v>
       </c>
       <c r="O13">
         <f>J9</f>
-        <v>276.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>283.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="46">
         <v>10</v>
       </c>
@@ -1676,7 +1695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="46">
         <v>11</v>
       </c>
@@ -1684,7 +1703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" s="46">
         <v>12</v>
       </c>
@@ -1692,26 +1711,38 @@
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>52</v>
+      </c>
+      <c r="Q16" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="63"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="46">
         <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="Q17" s="61">
+        <v>41275</v>
+      </c>
+      <c r="R17" s="17">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="46">
         <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18" s="13"/>
+      <c r="R18" s="18"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="46">
         <v>15</v>
       </c>
@@ -1731,7 +1762,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="25"/>
     </row>
-    <row r="20" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:18" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="49">
         <v>16</v>
       </c>
@@ -1740,7 +1771,7 @@
       </c>
       <c r="O20" s="26"/>
     </row>
-    <row r="21" spans="1:15" s="5" customFormat="1">
+    <row r="21" spans="1:18" s="5" customFormat="1">
       <c r="A21" s="47">
         <v>17</v>
       </c>
@@ -1749,114 +1780,113 @@
       </c>
       <c r="D21" s="5">
         <f>SUM(D10:D20)</f>
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" ref="E21:O21" si="5">SUM(E10:E20)</f>
-        <v>30333.289999999997</v>
+        <v>44100</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="5"/>
-        <v>39143.33</v>
+        <v>44100</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="5"/>
-        <v>39143.33</v>
+        <v>44100</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="5"/>
-        <v>39143.33</v>
+        <v>44100</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="5"/>
-        <v>39210.83</v>
+        <v>44100</v>
       </c>
       <c r="J21" s="5">
         <f>SUM(J10:J20)</f>
-        <v>54749.83</v>
+        <v>45535.25</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="5"/>
-        <v>40789.33</v>
+        <v>43283.5</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="5"/>
-        <v>40789.33</v>
+        <v>43283.5</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>40789.33</v>
+        <v>43283.5</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="5"/>
-        <v>40789.33</v>
+        <v>43283.5</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="5"/>
-        <v>41619.58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>43567</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="46">
         <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
-        <f>Hoja2!F4</f>
-        <v>3650</v>
+      <c r="C22" s="60">
+        <v>3700</v>
       </c>
       <c r="D22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="E22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="F22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="G22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="H22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="I22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="J22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="K22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="L22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="M22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="N22">
         <f>C22*7</f>
-        <v>25550</v>
+        <v>25900</v>
       </c>
       <c r="O22">
         <f>C22*7</f>
-        <v>25550</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="5" customFormat="1">
+        <v>25900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="5" customFormat="1">
       <c r="A23" s="47">
         <v>19</v>
       </c>
@@ -1865,131 +1895,131 @@
       </c>
       <c r="D23" s="39">
         <f>D21-D22</f>
-        <v>-25550</v>
+        <v>18200</v>
       </c>
       <c r="E23" s="5">
         <f>E21-E22</f>
-        <v>4783.2899999999972</v>
+        <v>18200</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ref="F23:O23" si="6">F21-F22</f>
-        <v>13593.330000000002</v>
+        <v>18200</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="6"/>
-        <v>13593.330000000002</v>
+        <v>18200</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="6"/>
-        <v>13593.330000000002</v>
+        <v>18200</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" si="6"/>
-        <v>13660.830000000002</v>
+        <v>18200</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="6"/>
-        <v>29199.83</v>
+        <v>19635.25</v>
       </c>
       <c r="K23" s="5">
         <f>K21-K22</f>
-        <v>15239.330000000002</v>
+        <v>17383.5</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="6"/>
-        <v>15239.330000000002</v>
+        <v>17383.5</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="6"/>
-        <v>15239.330000000002</v>
+        <v>17383.5</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="6"/>
-        <v>15239.330000000002</v>
+        <v>17383.5</v>
       </c>
       <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>16069.580000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>17667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="B24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="46">
         <v>20</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="37">
         <v>0.15</v>
       </c>
       <c r="D25" s="38">
         <f>IF(D23&gt;0,(D23*C25),0)</f>
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="E25" s="38">
         <f>IF(E23&gt;0,(E23*C25),0)</f>
-        <v>717.49349999999959</v>
+        <v>2730</v>
       </c>
       <c r="F25" s="38">
         <f>IF(F23&gt;0,(F23*C25),0)</f>
-        <v>2038.9995000000001</v>
+        <v>2730</v>
       </c>
       <c r="G25" s="38">
         <f>IF(G23&gt;0,(G23*C25),0)</f>
-        <v>2038.9995000000001</v>
+        <v>2730</v>
       </c>
       <c r="H25" s="38">
         <f>IF(H23&gt;0,(H23*C25),0)</f>
-        <v>2038.9995000000001</v>
+        <v>2730</v>
       </c>
       <c r="I25" s="38">
         <f>IF(I23&gt;0,(I23*C25),0)</f>
-        <v>2049.1245000000004</v>
+        <v>2730</v>
       </c>
       <c r="J25" s="38">
         <f>IF(J23&gt;0,(J23*C25),0)</f>
-        <v>4379.9745000000003</v>
+        <v>2945.2874999999999</v>
       </c>
       <c r="K25" s="38">
         <f>IF(K23&gt;0,(K23*C25),0)</f>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="L25" s="38">
         <f>IF(L23&gt;0,(L23*C25),0)</f>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="M25" s="38">
         <f>IF(M23&gt;0,(M23*C25),0)</f>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="N25" s="38">
         <f>IF(N23&gt;0,(N23*C25),0)</f>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="O25" s="38">
         <f>IF(O23&gt;0,(O23*C25),0)</f>
-        <v>2410.4370000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>2650.0499999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="B26" s="16"/>
       <c r="C26" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="23"/>
       <c r="O26"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:18">
       <c r="A27" s="46">
         <v>21</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="36">
         <v>0.21</v>
@@ -1997,133 +2027,133 @@
       <c r="D27" s="23"/>
       <c r="O27"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:18">
       <c r="B28" s="16"/>
       <c r="C28" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O28"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:18">
       <c r="A29" s="46">
         <v>22</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="36">
         <v>0.3</v>
       </c>
       <c r="D29" s="23"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1">
+    <row r="30" spans="1:18" s="1" customFormat="1">
       <c r="A30" s="46"/>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="1">
         <f>ROUND(D25+D27+D29,2)</f>
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="E30" s="1">
         <f>ROUND(E25,2)</f>
-        <v>717.49</v>
+        <v>2730</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ref="F30:M30" si="7">ROUND(F25,2)</f>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="7"/>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="7"/>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="7"/>
-        <v>2049.12</v>
+        <v>2730</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="7"/>
-        <v>4379.97</v>
+        <v>2945.29</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" si="7"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="7"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="M30" s="1">
         <f t="shared" si="7"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" ref="N30:O30" si="8">N25</f>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" si="8"/>
-        <v>2410.4370000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="1" customFormat="1">
+        <v>2650.0499999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="1" customFormat="1">
       <c r="A32" s="46">
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1">
         <f>D30</f>
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" ref="E32:O32" si="9">E30</f>
-        <v>717.49</v>
+        <f t="shared" ref="E32:N32" si="9">E30</f>
+        <v>2730</v>
       </c>
       <c r="F32" s="1">
         <f>F30</f>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="G32" s="1">
         <f>G30</f>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="9"/>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="9"/>
-        <v>2049.12</v>
+        <v>2730</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="9"/>
-        <v>4379.97</v>
+        <v>2945.29</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="9"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="9"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="M32" s="1">
         <f t="shared" si="9"/>
-        <v>2285.9</v>
+        <v>2607.5300000000002</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" si="9"/>
-        <v>2285.8995</v>
+        <v>2607.5250000000001</v>
       </c>
       <c r="O32" s="1">
         <f>O30</f>
-        <v>2410.4370000000004</v>
+        <v>2650.0499999999997</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2131,43 +2161,43 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G34" s="35">
         <f>ROUND(D37+E37+F37,2)</f>
-        <v>229.71</v>
+        <v>682.5</v>
       </c>
       <c r="H34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>430.74</v>
+        <v>910</v>
       </c>
       <c r="I34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>430.74</v>
+        <v>910</v>
       </c>
       <c r="J34" s="40">
         <f>ROUND((G34+G37),2)</f>
-        <v>430.74</v>
+        <v>910</v>
       </c>
       <c r="K34" s="42">
         <f>ROUND(G34+J34,2)</f>
-        <v>660.45</v>
+        <v>1592.5</v>
       </c>
       <c r="L34" s="31">
         <f>K34+K37</f>
-        <v>985.54</v>
+        <v>1795.51</v>
       </c>
       <c r="M34" s="31">
         <f>K34+K37</f>
-        <v>985.54</v>
+        <v>1795.51</v>
       </c>
       <c r="N34" s="31">
         <f>K34+K37</f>
-        <v>985.54</v>
+        <v>1795.51</v>
       </c>
       <c r="O34" s="43">
         <f>D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37</f>
-        <v>2628.08</v>
+        <v>2431.4499999999998</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="8" customFormat="1">
@@ -2175,55 +2205,55 @@
         <v>25</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="8">
         <f>D32</f>
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="E35" s="8">
         <f t="shared" ref="E35:F35" si="10">E32</f>
-        <v>717.49</v>
+        <v>2730</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="10"/>
-        <v>2039</v>
+        <v>2730</v>
       </c>
       <c r="G35" s="8">
         <f>ROUND(G32-G34,2)</f>
-        <v>1809.29</v>
+        <v>2047.5</v>
       </c>
       <c r="H35" s="8">
         <f>ROUND(H32-H34,2)</f>
-        <v>1608.26</v>
+        <v>1820</v>
       </c>
       <c r="I35" s="8">
         <f>ROUND(I32-I34,2)</f>
-        <v>1618.38</v>
+        <v>1820</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" ref="J35:O35" si="11">ROUND(J32-J34,2)</f>
-        <v>3949.23</v>
+        <f t="shared" ref="J35:M35" si="11">ROUND(J32-J34,2)</f>
+        <v>2035.29</v>
       </c>
       <c r="K35" s="8">
         <f>ROUND(K32-K34,2)</f>
-        <v>1625.45</v>
+        <v>1015.03</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" si="11"/>
-        <v>1300.3599999999999</v>
+        <v>812.02</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" si="11"/>
-        <v>1300.3599999999999</v>
+        <v>812.02</v>
       </c>
       <c r="N35" s="8">
         <f>ROUND(N32-N34,2)</f>
-        <v>1300.3599999999999</v>
+        <v>812.02</v>
       </c>
       <c r="O35" s="8">
         <f>ROUND(O34-O32,2)</f>
-        <v>217.64</v>
+        <v>-218.6</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="23" customFormat="1">
@@ -2231,7 +2261,7 @@
         <v>26</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" s="27">
         <v>12</v>
@@ -2275,55 +2305,55 @@
         <v>27</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="41">
         <f>ROUND(D35/D36,2)</f>
-        <v>0</v>
+        <v>227.5</v>
       </c>
       <c r="E37" s="41">
         <f>ROUND(E35/E36,2)</f>
-        <v>59.79</v>
+        <v>227.5</v>
       </c>
       <c r="F37" s="41">
         <f>ROUND(F35/F36,2)</f>
-        <v>169.92</v>
+        <v>227.5</v>
       </c>
       <c r="G37" s="24">
         <f>ROUND((G35/G36),2)</f>
-        <v>201.03</v>
+        <v>227.5</v>
       </c>
       <c r="H37" s="24">
         <f>ROUND((H35/H36),2)</f>
-        <v>201.03</v>
+        <v>227.5</v>
       </c>
       <c r="I37" s="24">
         <f>ROUND((I35/I36),2)</f>
-        <v>202.3</v>
+        <v>227.5</v>
       </c>
       <c r="J37" s="24">
         <f t="shared" ref="J37:O37" si="12">ROUND((J35/J36),2)</f>
-        <v>493.65</v>
+        <v>254.41</v>
       </c>
       <c r="K37" s="44">
         <f t="shared" si="12"/>
-        <v>325.08999999999997</v>
+        <v>203.01</v>
       </c>
       <c r="L37" s="24">
         <f t="shared" si="12"/>
-        <v>325.08999999999997</v>
+        <v>203.01</v>
       </c>
       <c r="M37" s="24">
         <f t="shared" si="12"/>
-        <v>325.08999999999997</v>
+        <v>203.01</v>
       </c>
       <c r="N37" s="24">
         <f t="shared" si="12"/>
-        <v>325.08999999999997</v>
+        <v>203.01</v>
       </c>
       <c r="O37" s="24">
         <f t="shared" si="12"/>
-        <v>217.64</v>
+        <v>-218.6</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2360,6 +2390,9 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="Q16:R16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2371,7 +2404,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2389,19 +2422,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="10">
         <v>0.15</v>
@@ -2415,7 +2448,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="10">
         <v>0.21</v>
@@ -2430,7 +2463,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="11">
         <v>0.3</v>

</xml_diff>